<commit_message>
se agrega documentacion de propuesta Experian
</commit_message>
<xml_diff>
--- a/Stefanini/Stefanini.Clientes/Stefanini.Clientes.UTP/diplomado.xlsx
+++ b/Stefanini/Stefanini.Clientes/Stefanini.Clientes.UTP/diplomado.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rene\Documents\Stefanini\Stefanini.Clientes\Stefanini.Clientes.UTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\omesan\Agile\Stefanini\Stefanini.Clientes\Stefanini.Clientes.UTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Fundamentos Agilismo</t>
   </si>
@@ -127,12 +127,6 @@
     <t>Feedback de evaluaciones</t>
   </si>
   <si>
-    <t>Ceremonias</t>
-  </si>
-  <si>
-    <t>Mapa de Historias de usuario</t>
-  </si>
-  <si>
     <t>Personal Maps</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>Simulación de la implantación de Scrum para el desarrollo de productos</t>
   </si>
   <si>
-    <t>Artefactos</t>
-  </si>
-  <si>
     <t>PRODUCT OWNER</t>
   </si>
   <si>
@@ -163,9 +154,6 @@
     <t>Mapa de Releases</t>
   </si>
   <si>
-    <t>Inceptión - Sprint 0 - Diferencias entre Inceptión y Sprint 0</t>
-  </si>
-  <si>
     <t>Evaluación de PO</t>
   </si>
   <si>
@@ -184,12 +172,6 @@
     <t>Líder Servicial - SM extraordinario</t>
   </si>
   <si>
-    <t>Estimación ágil - Gestión de impedimentos</t>
-  </si>
-  <si>
-    <t>Equipos de trabajo</t>
-  </si>
-  <si>
     <t>Radares ágiles</t>
   </si>
   <si>
@@ -208,9 +190,6 @@
     <t>Sprint 0</t>
   </si>
   <si>
-    <t>Diferencias entre Inceptión y Sprint 0</t>
-  </si>
-  <si>
     <t>Priorizando el Backlog de Producto</t>
   </si>
   <si>
@@ -226,23 +205,74 @@
     <t>Dinamica de creacion de Historias de Usuario</t>
   </si>
   <si>
-    <t>Roles</t>
-  </si>
-  <si>
     <t>Introducción a Scrum</t>
   </si>
   <si>
     <t>Kamban</t>
   </si>
   <si>
+    <t>Fundamentos Scrum</t>
+  </si>
+  <si>
+    <t>Roles de Scrum</t>
+  </si>
+  <si>
+    <t>Ceremonias de Scrum</t>
+  </si>
+  <si>
+    <t>Artefactos de Sscrum</t>
+  </si>
+  <si>
+    <t>Principios y valores de Scrum</t>
+  </si>
+  <si>
+    <t>Cynefin la complejidad que nos rodea</t>
+  </si>
+  <si>
+    <t>Visual story mapping en la practica</t>
+  </si>
+  <si>
     <t>Estimación ágil</t>
+  </si>
+  <si>
+    <t>Ejercicio de estimacion (planing poker)</t>
+  </si>
+  <si>
+    <t>Gestión de impedimentos</t>
+  </si>
+  <si>
+    <t>Equipos de alto rendimiento</t>
+  </si>
+  <si>
+    <t>Mejora continua</t>
+  </si>
+  <si>
+    <t>Taller de retrospectivas</t>
+  </si>
+  <si>
+    <t>Sprint Planning</t>
+  </si>
+  <si>
+    <t>Scrum diario</t>
+  </si>
+  <si>
+    <t>Sprint Review</t>
+  </si>
+  <si>
+    <t>Refinamiento del product backlog</t>
+  </si>
+  <si>
+    <t>Actividad Super Poderes</t>
+  </si>
+  <si>
+    <t>Toyota Kata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,13 +311,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF003245"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -385,9 +408,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -399,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -422,12 +443,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -437,6 +452,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -444,13 +471,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -793,10 +813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:M27"/>
+  <dimension ref="C1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19:L19"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +840,7 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -829,7 +849,7 @@
       <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -838,26 +858,26 @@
       <c r="L2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="11"/>
-      <c r="G3" s="8" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="11"/>
-      <c r="K3" s="8" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="9"/>
+      <c r="K3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="11"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
@@ -866,9 +886,7 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
@@ -895,9 +913,7 @@
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
@@ -924,9 +940,7 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
@@ -947,32 +961,32 @@
       </c>
     </row>
     <row r="7" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11"/>
-      <c r="G7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="11"/>
-      <c r="K7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="11"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="9"/>
+      <c r="G7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="9"/>
+      <c r="K7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="11">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9"/>
       <c r="G8" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H8" s="4">
         <v>1</v>
@@ -980,24 +994,26 @@
       <c r="I8" s="4">
         <v>1</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="4"/>
+      <c r="K8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
       <c r="M8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="G9" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H9" s="4">
         <v>1</v>
@@ -1005,24 +1021,26 @@
       <c r="I9" s="4">
         <v>1</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="4"/>
+      <c r="K9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
       <c r="M9" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
+      <c r="E10" s="4"/>
       <c r="G10" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
@@ -1030,80 +1048,86 @@
       <c r="I10" s="4">
         <v>1</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="4"/>
+      <c r="K10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1</v>
+      </c>
       <c r="M10" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="4"/>
       <c r="G11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="18">
-        <v>1</v>
-      </c>
-      <c r="I11" s="18">
+        <v>45</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="K11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="4">
         <v>2</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
-        <v>2</v>
-      </c>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="4">
-        <v>2</v>
-      </c>
+      <c r="E12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="18">
-        <v>1</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="K12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1</v>
+      </c>
       <c r="M12" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="G13" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="18">
-        <v>1</v>
-      </c>
-      <c r="I13" s="18">
-        <v>2</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7">
-        <v>2</v>
-      </c>
+      <c r="G13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="K13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="4">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
@@ -1112,21 +1136,23 @@
       <c r="D14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
+      <c r="E14" s="4"/>
       <c r="G14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="18">
-        <v>1</v>
-      </c>
-      <c r="I14" s="18">
-        <v>2</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="K14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
@@ -1135,22 +1161,22 @@
       <c r="D15" s="4">
         <v>1</v>
       </c>
-      <c r="E15" s="4">
-        <v>2</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="G15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="18">
-        <v>1</v>
-      </c>
-      <c r="I15" s="18">
-        <v>2</v>
-      </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="K15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
       <c r="M15" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1160,288 +1186,270 @@
       <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="7"/>
+      <c r="G16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="K16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="K17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="G18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="K18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" s="4">
         <v>2</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="18">
-        <v>1</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="12"/>
-      <c r="G17" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="18">
-        <v>1</v>
-      </c>
-      <c r="I17" s="18">
-        <v>2</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="4">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4">
-        <v>2</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="18">
-        <v>2</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7">
-        <v>3</v>
+      <c r="M18" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
       </c>
-      <c r="E19" s="4">
-        <v>3</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="G19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="18">
-        <v>1</v>
-      </c>
-      <c r="I19" s="18">
-        <v>3</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="12"/>
+        <v>52</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="K19" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
+      <c r="M19" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
-      <c r="E20" s="4">
-        <v>3</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="G20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" s="18">
-        <v>1</v>
-      </c>
-      <c r="I20" s="18">
-        <v>3</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4"/>
       <c r="K20" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
       </c>
       <c r="M20" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
       <c r="E21" s="4"/>
       <c r="G21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="18">
-        <v>1</v>
-      </c>
-      <c r="I21" s="18">
-        <v>3</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="4"/>
       <c r="K21" s="5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="L21" s="4">
         <v>1</v>
       </c>
-      <c r="M21" s="4">
-        <v>3</v>
-      </c>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
       <c r="E22" s="4"/>
       <c r="G22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="K22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="G23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="K23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2</v>
+      </c>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="4">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4">
-        <v>3</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L22" s="4">
-        <v>1</v>
-      </c>
-      <c r="M22" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="3:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4">
-        <v>3</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="7">
-        <v>1</v>
-      </c>
-      <c r="I23" s="7">
-        <v>3</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L23" s="4">
-        <v>1</v>
-      </c>
-      <c r="M23" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="3:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="G24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="12">
+        <v>1</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="K24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="7">
+        <v>1</v>
+      </c>
+      <c r="M24" s="7"/>
+    </row>
+    <row r="25" spans="3:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="7">
         <v>2</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="K24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L24" s="4">
-        <v>2</v>
-      </c>
-      <c r="M24" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="6" t="s">
+      <c r="E25" s="7"/>
+      <c r="K25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="7">
-        <v>1</v>
-      </c>
-      <c r="E25" s="7">
-        <v>3</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L25" s="4">
-        <v>1</v>
-      </c>
-      <c r="M25" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D26" s="4">
         <v>1</v>
       </c>
-      <c r="E26" s="4">
-        <v>3</v>
-      </c>
+      <c r="E26" s="4"/>
       <c r="H26">
         <f>SUM(H4:H25)</f>
-        <v>19</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L26" s="7">
-        <v>1</v>
-      </c>
-      <c r="M26" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <f>SUM(D4:D26)</f>
+        <v>20</v>
+      </c>
+      <c r="L26">
+        <f>SUM(L4:L25)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f>SUM(D4:D27)</f>
         <v>23</v>
       </c>
-      <c r="L27">
-        <f>SUM(L4:L26)</f>
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C7:D7"/>
+  <mergeCells count="7">
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1452,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,10 +1481,10 @@
       </c>
     </row>
     <row r="3" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
@@ -1503,10 +1511,10 @@
       </c>
     </row>
     <row r="7" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
@@ -1593,7 +1601,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1623,7 +1631,7 @@
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D22">
         <f>SUM(D8:D21)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se ajusta propuesta talleres UTP
</commit_message>
<xml_diff>
--- a/Stefanini/Stefanini.Clientes/Stefanini.Clientes.UTP/diplomado.xlsx
+++ b/Stefanini/Stefanini.Clientes/Stefanini.Clientes.UTP/diplomado.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Principios de Agilismo" sheetId="3" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="devops" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Fundamentos Agilismo</t>
   </si>
@@ -64,21 +64,9 @@
     <t>Historia de DevOps</t>
   </si>
   <si>
-    <t>Cultura</t>
-  </si>
-  <si>
     <t>Evaluación Introducción, Historia y Cultura</t>
   </si>
   <si>
-    <t>Organización</t>
-  </si>
-  <si>
-    <t>Procesos</t>
-  </si>
-  <si>
-    <t>Automatización</t>
-  </si>
-  <si>
     <t>Evaluación de Organización, Procesos y Automatización</t>
   </si>
   <si>
@@ -88,9 +76,6 @@
     <t>Integración continua</t>
   </si>
   <si>
-    <t>Depliegue</t>
-  </si>
-  <si>
     <t>Evaluación Métricas, Integración, Despliegue</t>
   </si>
   <si>
@@ -100,9 +85,6 @@
     <t>Herramientas de Automatizacion</t>
   </si>
   <si>
-    <t>Sesión</t>
-  </si>
-  <si>
     <t>AGILISMO</t>
   </si>
   <si>
@@ -266,13 +248,64 @@
   </si>
   <si>
     <t>Toyota Kata</t>
+  </si>
+  <si>
+    <t>Conceptos principales de DevOps</t>
+  </si>
+  <si>
+    <t>Introducción a la cultura DevOps</t>
+  </si>
+  <si>
+    <t>Elementos clave de DevOps</t>
+  </si>
+  <si>
+    <t>Implementación de una cultura DevOps</t>
+  </si>
+  <si>
+    <t>Modelos organizacionales</t>
+  </si>
+  <si>
+    <t>Equipos autónomos</t>
+  </si>
+  <si>
+    <t>Estilos de arquitectura</t>
+  </si>
+  <si>
+    <t>Optimización de procesos</t>
+  </si>
+  <si>
+    <t>Ciclo de vida de entrega de software en una organización DevOps</t>
+  </si>
+  <si>
+    <t>Automatización para la entrega de software</t>
+  </si>
+  <si>
+    <t>Conceptos clave de entrega continua</t>
+  </si>
+  <si>
+    <t>Conceptos de automatización de entrega continua</t>
+  </si>
+  <si>
+    <t>Control de Versiones</t>
+  </si>
+  <si>
+    <t>Desplieges continuos</t>
+  </si>
+  <si>
+    <t>Vision General de jenkins</t>
+  </si>
+  <si>
+    <t>Taller de contruccion de Flujo de Integracion Continua</t>
+  </si>
+  <si>
+    <t>Temas y actividades por sesiones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,13 +329,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="7"/>
-      <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -334,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -408,19 +434,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -443,34 +495,40 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -813,641 +871,530 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:M28"/>
+  <dimension ref="C1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="F10" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="62.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="59" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="F1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="I1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="I2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="J2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="14"/>
-      <c r="E3" s="9"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="9"/>
-      <c r="K3" s="13" t="s">
+      <c r="G3" s="14"/>
+      <c r="I3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="F7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="I7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="F17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="10">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="9"/>
-      <c r="G7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="9"/>
-      <c r="K7" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="G8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="4">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="4">
-        <v>1</v>
-      </c>
-      <c r="M8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="11" t="s">
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>SUM(G4:G25)</f>
+        <v>20</v>
+      </c>
+      <c r="J26">
+        <f>SUM(J4:J25)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="G9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="4">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4">
-        <v>1</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" s="4">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="G10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="4">
-        <v>1</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="4">
-        <v>1</v>
-      </c>
-      <c r="M10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="G11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="K11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="4">
-        <v>2</v>
-      </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="G12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="K12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="4">
-        <v>1</v>
-      </c>
-      <c r="M12" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="G13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="4">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4"/>
-      <c r="K13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="4">
-        <v>1</v>
-      </c>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="G14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="4">
-        <v>1</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="K14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1</v>
-      </c>
-      <c r="M14" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="G15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-      <c r="I15" s="4"/>
-      <c r="K15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1</v>
-      </c>
-      <c r="M15" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="7">
-        <v>1</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="G16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="4">
-        <v>1</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="K16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1</v>
-      </c>
-      <c r="M16" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="10"/>
-      <c r="G17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="4">
-        <v>1</v>
-      </c>
-      <c r="I17" s="4"/>
-      <c r="K17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L17" s="4">
-        <v>1</v>
-      </c>
-      <c r="M17" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="G18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="4">
-        <v>1</v>
-      </c>
-      <c r="I18" s="4"/>
-      <c r="K18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L18" s="4">
-        <v>2</v>
-      </c>
-      <c r="M18" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="G19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="K19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L19" s="4">
-        <v>1</v>
-      </c>
-      <c r="M19" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="G20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="4">
-        <v>1</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="K20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L20" s="4">
-        <v>1</v>
-      </c>
-      <c r="M20" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="G21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="4">
-        <v>1</v>
-      </c>
-      <c r="I21" s="4"/>
-      <c r="K21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L21" s="4">
-        <v>1</v>
-      </c>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="G22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H22" s="4">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4"/>
-      <c r="K22" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L22" s="4">
-        <v>1</v>
-      </c>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="G23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="7">
-        <v>1</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="K23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L23" s="4">
-        <v>2</v>
-      </c>
-      <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="G24" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="12">
-        <v>1</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="K24" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L24" s="7">
-        <v>1</v>
-      </c>
-      <c r="M24" s="7"/>
-    </row>
-    <row r="25" spans="3:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="7">
-        <v>2</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="K25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L25" s="4">
-        <v>1</v>
-      </c>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="H26">
-        <f>SUM(H4:H25)</f>
-        <v>20</v>
-      </c>
-      <c r="L26">
-        <f>SUM(L4:L25)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="D28">
-        <f>SUM(D4:D27)</f>
-        <v>23</v>
+      <c r="D27" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C7:D7"/>
   </mergeCells>
@@ -1458,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D22"/>
+  <dimension ref="C1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,12 +1418,17 @@
     <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="18"/>
+    </row>
     <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1526,7 +1478,7 @@
     </row>
     <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1534,23 +1486,23 @@
     </row>
     <row r="10" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1558,39 +1510,39 @@
     </row>
     <row r="13" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="5" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="D15" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="5" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -1598,46 +1550,137 @@
     </row>
     <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="5" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="D18" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="7">
+      <c r="C20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D22">
-        <f>SUM(D8:D21)</f>
+    <row r="22" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
se ajusta presentaciones Experian
</commit_message>
<xml_diff>
--- a/Stefanini/Stefanini.Clientes/Stefanini.Clientes.UTP/diplomado.xlsx
+++ b/Stefanini/Stefanini.Clientes/Stefanini.Clientes.UTP/diplomado.xlsx
@@ -100,9 +100,6 @@
     <t>Evaluación de Agilismo</t>
   </si>
   <si>
-    <t>SCRUM</t>
-  </si>
-  <si>
     <t>Evaluación de fundamentos SCRUM</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Temas y actividades por sesiones</t>
+  </si>
+  <si>
+    <t>SCRUM COMO MARCO DE TRABAJO</t>
   </si>
 </sst>
 </file>
@@ -504,31 +504,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -873,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView topLeftCell="D9" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J25"/>
     </sheetView>
   </sheetViews>
@@ -889,17 +889,17 @@
   <sheetData>
     <row r="1" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="14"/>
       <c r="F1" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G1" s="16"/>
-      <c r="I1" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="18"/>
+      <c r="I1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
@@ -914,10 +914,10 @@
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1001,29 +1001,29 @@
       </c>
       <c r="D7" s="14"/>
       <c r="F7" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="I7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="12"/>
+      <c r="I7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J8" s="4">
         <v>1</v>
@@ -1037,13 +1037,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" s="4">
         <v>1</v>
@@ -1051,19 +1051,19 @@
     </row>
     <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="4">
         <v>1</v>
@@ -1071,19 +1071,19 @@
     </row>
     <row r="11" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="4">
         <v>1</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J11" s="4">
         <v>2</v>
@@ -1091,19 +1091,19 @@
     </row>
     <row r="12" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G12" s="4">
         <v>1</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12" s="4">
         <v>1</v>
@@ -1111,19 +1111,19 @@
     </row>
     <row r="13" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J13" s="4">
         <v>1</v>
@@ -1137,13 +1137,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J14" s="4">
         <v>1</v>
@@ -1157,13 +1157,13 @@
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J15" s="4">
         <v>1</v>
@@ -1177,31 +1177,31 @@
         <v>1</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G16" s="4">
         <v>1</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J16" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="12"/>
+      <c r="C17" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="19"/>
       <c r="F17" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J17" s="4">
         <v>1</v>
@@ -1209,19 +1209,19 @@
     </row>
     <row r="18" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="4">
         <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J18" s="4">
         <v>2</v>
@@ -1229,19 +1229,19 @@
     </row>
     <row r="19" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" s="4">
         <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J19" s="4">
         <v>1</v>
@@ -1249,19 +1249,19 @@
     </row>
     <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4">
         <v>1</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J20" s="4">
         <v>1</v>
@@ -1269,19 +1269,19 @@
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G21" s="4">
         <v>1</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J21" s="4">
         <v>1</v>
@@ -1289,19 +1289,19 @@
     </row>
     <row r="22" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="4">
         <v>1</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J22" s="4">
         <v>1</v>
@@ -1309,19 +1309,19 @@
     </row>
     <row r="23" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="7">
         <v>1</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="4">
         <v>2</v>
@@ -1329,19 +1329,19 @@
     </row>
     <row r="24" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J24" s="7">
         <v>1</v>
@@ -1349,13 +1349,13 @@
     </row>
     <row r="25" spans="3:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J25" s="4">
         <v>1</v>
@@ -1363,23 +1363,15 @@
     </row>
     <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
-      </c>
-      <c r="G26">
-        <f>SUM(G4:G25)</f>
-        <v>20</v>
-      </c>
-      <c r="J26">
-        <f>SUM(J4:J25)</f>
-        <v>24</v>
       </c>
     </row>
     <row r="27" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -1407,7 +1399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:D33"/>
     </sheetView>
   </sheetViews>
@@ -1419,16 +1411,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C1" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="18"/>
+      <c r="C1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1478,7 +1470,7 @@
     </row>
     <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1494,7 +1486,7 @@
     </row>
     <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -1502,7 +1494,7 @@
     </row>
     <row r="12" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1510,7 +1502,7 @@
     </row>
     <row r="13" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -1526,7 +1518,7 @@
     </row>
     <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -1534,7 +1526,7 @@
     </row>
     <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -1542,7 +1534,7 @@
     </row>
     <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -1550,7 +1542,7 @@
     </row>
     <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1558,7 +1550,7 @@
     </row>
     <row r="19" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -1566,7 +1558,7 @@
     </row>
     <row r="20" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -1574,7 +1566,7 @@
     </row>
     <row r="21" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -1582,7 +1574,7 @@
     </row>
     <row r="22" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -1598,7 +1590,7 @@
     </row>
     <row r="24" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -1622,7 +1614,7 @@
     </row>
     <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -1630,7 +1622,7 @@
     </row>
     <row r="28" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
@@ -1646,7 +1638,7 @@
     </row>
     <row r="30" spans="3:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="4">
         <v>4</v>
@@ -1670,7 +1662,7 @@
     </row>
     <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>

</xml_diff>